<commit_message>
03 classification validation & restructure future labs
</commit_message>
<xml_diff>
--- a/Microsoft/Purview/Purview-Retail-Data-Protection-Masterclass/02-Data-Foundation/data-templates/Banking-DirectDeposit.xlsx
+++ b/Microsoft/Purview/Purview-Retail-Data-Protection-Masterclass/02-Data-Foundation/data-templates/Banking-DirectDeposit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPO\GitHub\Projects\Microsoft\Purview\Purview-Retail-Data-Protection-Masterclass\02-Data-Foundation\data-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ECB9511-B535-44A4-91D6-87662FF00FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9198562-8CF3-4CC8-A123-F1911883AAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1CDAAE19-7D9E-44D3-9D5C-6BBC6AEF8558}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EE8AE95E-5C65-43A4-8BED-EE10421DDC8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct Deposit" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Customer ID</t>
   </si>
@@ -59,121 +59,127 @@
     <t>C001</t>
   </si>
   <si>
+    <t>Lauren</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>lauren.smith@contoso.com</t>
+  </si>
+  <si>
+    <t>C002</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>robert.rodriguez@contoso.com</t>
+  </si>
+  <si>
+    <t>C003</t>
+  </si>
+  <si>
+    <t>lauren.smith@gmail.com</t>
+  </si>
+  <si>
+    <t>C004</t>
+  </si>
+  <si>
     <t>Amanda</t>
   </si>
   <si>
-    <t>Rodriguez</t>
-  </si>
-  <si>
-    <t>amanda.rodriguez@contoso.com</t>
-  </si>
-  <si>
-    <t>C002</t>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>amanda.wilson@contoso.com</t>
+  </si>
+  <si>
+    <t>C005</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>jessica.moore@contoso.com</t>
+  </si>
+  <si>
+    <t>C006</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>lauren.davis@hotmail.com</t>
+  </si>
+  <si>
+    <t>C007</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>emily.davis@contoso.com</t>
+  </si>
+  <si>
+    <t>C008</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>jennifer.gonzalez@contoso.com</t>
+  </si>
+  <si>
+    <t>C009</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>michael.taylor@icloud.com</t>
+  </si>
+  <si>
+    <t>C010</t>
   </si>
   <si>
     <t>Michelle</t>
   </si>
   <si>
-    <t>Moore</t>
-  </si>
-  <si>
-    <t>michelle.moore@contoso.com</t>
-  </si>
-  <si>
-    <t>C003</t>
-  </si>
-  <si>
-    <t>Daniel</t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
-    <t>daniel.williams@hotmail.com</t>
-  </si>
-  <si>
-    <t>C004</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Wilson</t>
-  </si>
-  <si>
-    <t>william.wilson@contoso.com</t>
-  </si>
-  <si>
-    <t>C005</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>william.taylor@contoso.com</t>
-  </si>
-  <si>
-    <t>C006</t>
-  </si>
-  <si>
-    <t>Jennifer</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>jennifer.martin@hotmail.com</t>
-  </si>
-  <si>
-    <t>C007</t>
-  </si>
-  <si>
-    <t>Michael</t>
-  </si>
-  <si>
-    <t>michael.moore@contoso.com</t>
-  </si>
-  <si>
-    <t>C008</t>
-  </si>
-  <si>
-    <t>Lisa</t>
-  </si>
-  <si>
-    <t>lisa.wilson@contoso.com</t>
-  </si>
-  <si>
-    <t>C009</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>amanda.martinez@hotmail.com</t>
-  </si>
-  <si>
-    <t>C010</t>
-  </si>
-  <si>
-    <t>Ashley</t>
-  </si>
-  <si>
-    <t>ashley.williams@contoso.com</t>
+    <t>michelle.taylor@contoso.com</t>
   </si>
   <si>
     <t>C011</t>
   </si>
   <si>
-    <t>william.martin@contoso.com</t>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>sarah.wilson@contoso.com</t>
   </si>
   <si>
     <t>C012</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>john.martin@hotmail.com</t>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>james.garcia@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A7BDB9-6638-41A8-84C1-C3638ED9C057}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F76F891-DF42-44C5-B4EB-C29493468744}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -571,7 +577,7 @@
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -605,10 +611,10 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>145557876</v>
+        <v>212524838</v>
       </c>
       <c r="E2">
-        <v>78634951</v>
+        <v>35928397</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -625,10 +631,10 @@
         <v>12</v>
       </c>
       <c r="D3">
-        <v>841347377</v>
+        <v>310308176</v>
       </c>
       <c r="E3">
-        <v>95257136</v>
+        <v>10080973</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -639,136 +645,136 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>661028505</v>
+      </c>
+      <c r="E4">
+        <v>69775754</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>353857665</v>
-      </c>
-      <c r="E4">
-        <v>71381734</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5">
+        <v>708747422</v>
+      </c>
+      <c r="E5">
+        <v>98891132</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>573257311</v>
-      </c>
-      <c r="E5">
-        <v>73621026</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6">
+        <v>344512868</v>
+      </c>
+      <c r="E6">
+        <v>23012863</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
-      </c>
-      <c r="D6">
-        <v>871025760</v>
-      </c>
-      <c r="E6">
-        <v>88850471</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7">
+        <v>42683438</v>
+      </c>
+      <c r="E7">
+        <v>85398874</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7">
-        <v>888237147</v>
-      </c>
-      <c r="E7">
-        <v>84404533</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>36667545</v>
+      </c>
+      <c r="E8">
+        <v>64007205</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>376760508</v>
-      </c>
-      <c r="E8">
-        <v>33333373</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9">
+        <v>770642858</v>
+      </c>
+      <c r="E9">
+        <v>94141095</v>
+      </c>
+      <c r="F9" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>357485081</v>
-      </c>
-      <c r="E9">
-        <v>33242581</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
       </c>
       <c r="D10">
-        <v>612462472</v>
+        <v>843461418</v>
       </c>
       <c r="E10">
-        <v>34098963</v>
+        <v>89235880</v>
       </c>
       <c r="F10" t="s">
         <v>37</v>
@@ -782,13 +788,13 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D11">
-        <v>474285260</v>
+        <v>256177166</v>
       </c>
       <c r="E11">
-        <v>62116979</v>
+        <v>54917528</v>
       </c>
       <c r="F11" t="s">
         <v>40</v>
@@ -799,39 +805,39 @@
         <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D12">
-        <v>54222057</v>
+        <v>152723520</v>
       </c>
       <c r="E12">
-        <v>62371167</v>
+        <v>25703299</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D13">
-        <v>137221825</v>
+        <v>116057488</v>
       </c>
       <c r="E13">
-        <v>28850061</v>
+        <v>54053051</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>